<commit_message>
#8 : adding trainings graphs
</commit_message>
<xml_diff>
--- a/Data/Documentation/Merged data set - Labelling.xlsx
+++ b/Data/Documentation/Merged data set - Labelling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb501238\Documents\GitHub\ReplicableResearch\Data\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899EC3B9-9BD0-4A53-B87E-EF6DF9236C15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE3C1B4-6935-4D35-BFC6-1649EF6C7F31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2357" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2361" uniqueCount="417">
   <si>
     <t>name</t>
   </si>
@@ -1171,21 +1171,6 @@
     <t>Projects went through external code review</t>
   </si>
   <si>
-    <t>Was trained in version control</t>
-  </si>
-  <si>
-    <t>Was trained in data management</t>
-  </si>
-  <si>
-    <t>Was trained in code automation</t>
-  </si>
-  <si>
-    <t>Was trained in coding practices</t>
-  </si>
-  <si>
-    <t>Wasn't trained in any of the tools</t>
-  </si>
-  <si>
     <t>Availability of resources on data management</t>
   </si>
   <si>
@@ -1262,6 +1247,39 @@
   </si>
   <si>
     <t>Masters</t>
+  </si>
+  <si>
+    <t>PI was trained in version control</t>
+  </si>
+  <si>
+    <t>PI was trained in data management</t>
+  </si>
+  <si>
+    <t>PI was trained in code automation</t>
+  </si>
+  <si>
+    <t>PI was trained in coding practices</t>
+  </si>
+  <si>
+    <t>PI wasn't trained in any of the tools</t>
+  </si>
+  <si>
+    <t>RA was trained in version control</t>
+  </si>
+  <si>
+    <t>RA was trained in data management</t>
+  </si>
+  <si>
+    <t>RA was trained in code automation</t>
+  </si>
+  <si>
+    <t>RA was trained in coding practices</t>
+  </si>
+  <si>
+    <t>RA wasn't trained in any of the tools</t>
+  </si>
+  <si>
+    <t>Does not know if RA was trained in any of the tools</t>
   </si>
 </sst>
 </file>
@@ -1622,8 +1640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="C151" sqref="C151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2835,7 +2853,7 @@
         <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="C44" t="s">
         <v>20</v>
@@ -3304,7 +3322,7 @@
         <v>80</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="C61" t="s">
         <v>20</v>
@@ -3362,7 +3380,7 @@
         <v>82</v>
       </c>
       <c r="B63" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="C63" t="s">
         <v>20</v>
@@ -3420,7 +3438,7 @@
         <v>84</v>
       </c>
       <c r="B65" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="C65" t="s">
         <v>20</v>
@@ -3478,7 +3496,7 @@
         <v>86</v>
       </c>
       <c r="B67" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="C67" t="s">
         <v>20</v>
@@ -3886,7 +3904,7 @@
         <v>101</v>
       </c>
       <c r="B82" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="C82" t="s">
         <v>20</v>
@@ -4141,7 +4159,7 @@
         <v>110</v>
       </c>
       <c r="B91" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="C91" t="s">
         <v>20</v>
@@ -4199,7 +4217,7 @@
         <v>112</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>380</v>
+        <v>406</v>
       </c>
       <c r="C93" t="s">
         <v>20</v>
@@ -4228,7 +4246,7 @@
         <v>113</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>381</v>
+        <v>407</v>
       </c>
       <c r="C94" t="s">
         <v>20</v>
@@ -4257,7 +4275,7 @@
         <v>114</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>382</v>
+        <v>408</v>
       </c>
       <c r="C95" t="s">
         <v>20</v>
@@ -4286,7 +4304,7 @@
         <v>115</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>383</v>
+        <v>409</v>
       </c>
       <c r="C96" t="s">
         <v>20</v>
@@ -4315,7 +4333,7 @@
         <v>116</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>384</v>
+        <v>410</v>
       </c>
       <c r="C97" t="s">
         <v>20</v>
@@ -4489,7 +4507,7 @@
         <v>122</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="C103" t="s">
         <v>20</v>
@@ -4602,7 +4620,7 @@
         <v>126</v>
       </c>
       <c r="B107" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="C107" t="s">
         <v>20</v>
@@ -4629,7 +4647,7 @@
         <v>127</v>
       </c>
       <c r="B108" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="C108" t="s">
         <v>20</v>
@@ -4656,7 +4674,7 @@
         <v>128</v>
       </c>
       <c r="B109" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="C109" t="s">
         <v>20</v>
@@ -4683,7 +4701,7 @@
         <v>129</v>
       </c>
       <c r="B110" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="C110" t="s">
         <v>20</v>
@@ -4710,7 +4728,7 @@
         <v>130</v>
       </c>
       <c r="B111" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="C111" t="s">
         <v>20</v>
@@ -4737,7 +4755,7 @@
         <v>131</v>
       </c>
       <c r="B112" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="C112" t="s">
         <v>20</v>
@@ -4764,7 +4782,7 @@
         <v>132</v>
       </c>
       <c r="B113" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C113" t="s">
         <v>20</v>
@@ -5049,7 +5067,7 @@
         <v>142</v>
       </c>
       <c r="B123" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="C123" t="s">
         <v>20</v>
@@ -5078,7 +5096,7 @@
         <v>143</v>
       </c>
       <c r="B124" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="C124" t="s">
         <v>20</v>
@@ -5278,7 +5296,7 @@
         <v>150</v>
       </c>
       <c r="B131" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="C131" t="s">
         <v>20</v>
@@ -5364,8 +5382,8 @@
       <c r="A134" t="s">
         <v>153</v>
       </c>
-      <c r="B134" t="s">
-        <v>20</v>
+      <c r="B134" s="1" t="s">
+        <v>411</v>
       </c>
       <c r="C134" t="s">
         <v>20</v>
@@ -5393,8 +5411,8 @@
       <c r="A135" t="s">
         <v>154</v>
       </c>
-      <c r="B135" t="s">
-        <v>20</v>
+      <c r="B135" s="1" t="s">
+        <v>412</v>
       </c>
       <c r="C135" t="s">
         <v>20</v>
@@ -5422,8 +5440,8 @@
       <c r="A136" t="s">
         <v>155</v>
       </c>
-      <c r="B136" t="s">
-        <v>20</v>
+      <c r="B136" s="1" t="s">
+        <v>413</v>
       </c>
       <c r="C136" t="s">
         <v>20</v>
@@ -5451,8 +5469,8 @@
       <c r="A137" t="s">
         <v>156</v>
       </c>
-      <c r="B137" t="s">
-        <v>20</v>
+      <c r="B137" s="1" t="s">
+        <v>414</v>
       </c>
       <c r="C137" t="s">
         <v>20</v>
@@ -5480,8 +5498,8 @@
       <c r="A138" t="s">
         <v>157</v>
       </c>
-      <c r="B138" t="s">
-        <v>20</v>
+      <c r="B138" s="1" t="s">
+        <v>415</v>
       </c>
       <c r="C138" t="s">
         <v>20</v>
@@ -5509,8 +5527,8 @@
       <c r="A139" t="s">
         <v>158</v>
       </c>
-      <c r="B139" t="s">
-        <v>20</v>
+      <c r="B139" s="1" t="s">
+        <v>416</v>
       </c>
       <c r="C139" t="s">
         <v>20</v>
@@ -5768,7 +5786,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -5790,7 +5808,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -5801,7 +5819,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -5823,7 +5841,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -5834,7 +5852,7 @@
         <v>232</v>
       </c>
       <c r="C13" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -5845,7 +5863,7 @@
         <v>233</v>
       </c>
       <c r="C14" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -5856,7 +5874,7 @@
         <v>234</v>
       </c>
       <c r="C15" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -5878,7 +5896,7 @@
         <v>232</v>
       </c>
       <c r="C17" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -5901,8 +5919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C353"/>
   <sheetViews>
-    <sheetView topLeftCell="A325" workbookViewId="0">
-      <selection activeCell="C351" sqref="A351:C353"/>
+    <sheetView topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="F348" sqref="F348"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Blog post: commit to change computers
</commit_message>
<xml_diff>
--- a/Data/Documentation/Merged data set - Labelling.xlsx
+++ b/Data/Documentation/Merged data set - Labelling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb501238\Documents\GitHub\ReplicableResearch\Data\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE3C1B4-6935-4D35-BFC6-1649EF6C7F31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334D46BA-34A2-4D4C-8FB3-08394F4D8C74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2361" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2356" uniqueCount="418">
   <si>
     <t>name</t>
   </si>
@@ -1280,6 +1280,9 @@
   </si>
   <si>
     <t>Does not know if RA was trained in any of the tools</t>
+  </si>
+  <si>
+    <t>Task management tool: Other, specify</t>
   </si>
 </sst>
 </file>
@@ -1640,8 +1643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="C151" sqref="C151"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2338,10 +2341,10 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" t="s">
-        <v>20</v>
+        <v>44</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>417</v>
       </c>
       <c r="C25" t="s">
         <v>20</v>
@@ -2367,9 +2370,6 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" t="s">
         <v>20</v>
       </c>
       <c r="C26" t="s">

</xml_diff>